<commit_message>
datepicker issue + banner
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\eao\beta\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38999C06-5EB5-41CC-AE4B-CB4C7D451EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B0287-E8AA-45EF-A6D7-02CA5DC47C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{296960FE-C65C-4E22-ABB9-815D3FEB7325}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2335" uniqueCount="381">
   <si>
     <t>Cell Colors</t>
   </si>
@@ -1321,9 +1321,6 @@
   </si>
   <si>
     <t>{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "event_name": "Last Day of EAC Assessment Readiness Decision (Date Capture Milestone)" }</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Revised Readiness Decision","work_type_id": 6, "ea_act_id": 3, "event_name": "Detailed Project Description Received", "start_at": 1 }</t>
   </si>
   <si>
     <t>[{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised DPD Development (Proponent Time)", "legislated": false },{"phase_name":"Readiness Decision","work_type_id": 6, "ea_act_id": 3, "new_name": "Revised Readiness Decision", "legislated": false }]</t>
@@ -18470,10 +18467,10 @@
   <dimension ref="A1:G290"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A122" sqref="A122:XFD122"/>
+      <selection pane="bottomRight" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18550,10 +18547,10 @@
         <v>253</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -19318,10 +19315,10 @@
         <v>253</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G35" s="3">
         <v>36</v>
@@ -19777,7 +19774,7 @@
         <v>280</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G54" s="3">
         <v>56</v>
@@ -19801,7 +19798,7 @@
         <v>261</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G55" s="3">
         <v>58</v>
@@ -19849,7 +19846,7 @@
         <v>282</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G57" s="3">
         <v>60</v>
@@ -19870,10 +19867,10 @@
         <v>253</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G58" s="3">
         <v>61</v>
@@ -20257,7 +20254,7 @@
         <v>287</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G74" s="3">
         <v>79</v>
@@ -20497,7 +20494,7 @@
         <v>280</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G84" s="3">
         <v>89</v>
@@ -20521,7 +20518,7 @@
         <v>261</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G85" s="3">
         <v>91</v>
@@ -20878,10 +20875,10 @@
         <v>253</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G100" s="3">
         <v>108</v>
@@ -21382,10 +21379,10 @@
         <v>253</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G121" s="3">
         <v>130</v>

</xml_diff>

<commit_message>
template fixes and change_phase_end_event action changes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08BAA25-8016-4D80-8F37-BFA98CAB2D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12945" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -20,7 +26,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$N$319</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outcomes!$A$1:$E$62</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1027,12 +1046,6 @@
     <t>ChangePhaseEndEvent</t>
   </si>
   <si>
-    <t>Set "Early Engagement | Project Transitioning FROM the EA Act (2002)" to PHASE END EVENT</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "Project Transitioning FROM the EA Act (2002)"}</t>
-  </si>
-  <si>
     <t>Set "DPD Development (Proponent Time) | Start of Detailed Project Description Development" ACTUAL to thisEventActual +1</t>
   </si>
   <si>
@@ -1376,19 +1389,19 @@
   </si>
   <si>
     <t>We currently don’t know how to handle this in EPIC.track</t>
+  </si>
+  <si>
+    <t>Set "Pre-Early Engagement | Project Transitioning FROM the EA Act (2002)" to PHASE END EVENT</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Pre-Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "Project Transitioning FROM the EA Act (2002)"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="27">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1426,150 +1439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1595,7 +1464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1604,19 +1473,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,13 +1497,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1667,170 +1536,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1882,253 +1589,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2261,65 +1726,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color theme="0"/>
       </font>
@@ -2329,28 +1758,19 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00CCFFCC"/>
+      <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2608,26 +2028,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.799981688894314"/>
+    <tabColor theme="9" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.62857142857143" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="21" spans="2:2">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
@@ -2650,62 +2069,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="21" spans="2:2">
+    <row r="8" spans="2:3" ht="21">
       <c r="B8" s="44" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" ht="21" spans="2:2">
+    <row r="12" spans="2:3" ht="21">
       <c r="B12" s="44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6285714285714" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="8" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6285714285714" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6328125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="12.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:9">
+    <row r="1" spans="1:9" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -3082,15 +2498,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:9">
       <c r="A14"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:9">
       <c r="A15"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:9">
       <c r="A16"/>
       <c r="B16"/>
     </row>
@@ -3863,51 +3279,61 @@
       <c r="B208"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13">
-      <formula1>Lookups!$B$3:$B$16</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
-      <formula1>Lookups!$D$3:$D$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13">
-      <formula1>Lookups!$F$3:$F$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$B$3:$B$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$D$3:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$F$3:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D164" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10.6285714285714" style="2" customWidth="1"/>
-    <col min="4" max="4" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6285714285714" style="1" customWidth="1"/>
-    <col min="7" max="9" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6285714285714" style="1" customWidth="1"/>
-    <col min="11" max="12" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6285714285714" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6328125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="14.6328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="14.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:14">
+    <row r="1" spans="1:14" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -8262,7 +7688,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="101" ht="15.75" spans="1:14">
+    <row r="101" spans="1:14">
       <c r="A101" s="2">
         <v>102</v>
       </c>
@@ -8347,7 +7773,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="103" ht="15.75" spans="1:14">
+    <row r="103" spans="1:14">
       <c r="A103" s="28">
         <v>104</v>
       </c>
@@ -9347,7 +8773,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="126" ht="15.75" spans="1:14">
+    <row r="126" spans="1:14">
       <c r="A126" s="2">
         <v>127</v>
       </c>
@@ -9389,7 +8815,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" ht="15.75" spans="1:14">
+    <row r="127" spans="1:14">
       <c r="A127" s="34">
         <v>128</v>
       </c>
@@ -17821,65 +17247,82 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N319">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:N319" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="H1:H319">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="between" text="END">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="between" text="START">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="START">
       <formula>NOT(ISERROR(SEARCH("START",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C319">
-      <formula1>Phases!$A$2:$A$13</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H319">
-      <formula1>Lookups!$Q$3:$Q$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F319">
-      <formula1>Lookups!$I$3:$I$39</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I319">
-      <formula1>Lookups!$S$3:$S$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G319">
-      <formula1>Lookups!$K$3:$K$9</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M319">
-      <formula1>Lookups!$M$3:$M$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Phases!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$Q$3:$Q$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$I$3:$I$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$S$3:$S$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$K$3:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000005000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$M$3:$M$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M319</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="4" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="70.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -18995,45 +18438,47 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E62">
-    <extLst/>
-  </autoFilter>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B62">
-      <formula1>Events!$A$2:$A$319</formula1>
-    </dataValidation>
-  </dataValidations>
+  <autoFilter ref="A1:E62" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Events!$A$2:$A$319</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B62</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.90476190476191" style="1"/>
-    <col min="2" max="2" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="108.628571428571" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="12.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="108.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -19167,10 +18612,10 @@
         <v>270</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G6" s="2">
         <v>7</v>
@@ -19191,10 +18636,10 @@
         <v>258</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="2">
         <v>8</v>
@@ -19215,10 +18660,10 @@
         <v>264</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G8" s="2">
         <v>9</v>
@@ -19239,10 +18684,10 @@
         <v>258</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G9" s="2">
         <v>10</v>
@@ -19263,10 +18708,10 @@
         <v>258</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G10" s="2">
         <v>11</v>
@@ -19287,10 +18732,10 @@
         <v>264</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G11" s="2">
         <v>12</v>
@@ -19335,10 +18780,10 @@
         <v>270</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G13" s="2">
         <v>14</v>
@@ -19359,10 +18804,10 @@
         <v>258</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G14" s="2">
         <v>15</v>
@@ -19383,10 +18828,10 @@
         <v>264</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G15" s="2">
         <v>16</v>
@@ -19431,10 +18876,10 @@
         <v>270</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G17" s="2">
         <v>18</v>
@@ -19455,10 +18900,10 @@
         <v>258</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G18" s="2">
         <v>19</v>
@@ -19479,10 +18924,10 @@
         <v>264</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G19" s="2">
         <v>20</v>
@@ -19503,10 +18948,10 @@
         <v>267</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G20" s="2">
         <v>21</v>
@@ -19524,13 +18969,13 @@
         <v>Proponent withdraws Submission from the EAC Assessment process</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G21" s="2">
         <v>22</v>
@@ -19548,13 +18993,13 @@
         <v>Proponent withdraws Submission from the EAC Assessment process</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G22" s="2">
         <v>23</v>
@@ -19572,13 +19017,13 @@
         <v>Starts the "clock" for EAC Assessment</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="G23" s="2">
         <v>24</v>
@@ -19596,13 +19041,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G24" s="2">
         <v>25</v>
@@ -19623,10 +19068,10 @@
         <v>264</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G25" s="2">
         <v>26</v>
@@ -19647,10 +19092,10 @@
         <v>267</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G26" s="2">
         <v>27</v>
@@ -19668,13 +19113,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G27" s="2">
         <v>28</v>
@@ -19692,13 +19137,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G28" s="2">
         <v>29</v>
@@ -19719,10 +19164,10 @@
         <v>264</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G29" s="2">
         <v>30</v>
@@ -19743,10 +19188,10 @@
         <v>267</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G30" s="2">
         <v>31</v>
@@ -19764,13 +19209,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G31" s="2">
         <v>32</v>
@@ -19788,13 +19233,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G32" s="2">
         <v>33</v>
@@ -19815,10 +19260,10 @@
         <v>258</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G33" s="2">
         <v>34</v>
@@ -19839,10 +19284,10 @@
         <v>258</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G34" s="2">
         <v>35</v>
@@ -19863,10 +19308,10 @@
         <v>261</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G35" s="2">
         <v>36</v>
@@ -19884,13 +19329,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G36" s="2">
         <v>38</v>
@@ -19911,10 +19356,10 @@
         <v>264</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G37" s="2">
         <v>39</v>
@@ -19935,10 +19380,10 @@
         <v>267</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G38" s="2">
         <v>40</v>
@@ -19956,13 +19401,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G39" s="2">
         <v>41</v>
@@ -19980,13 +19425,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G40" s="2">
         <v>42</v>
@@ -20007,10 +19452,10 @@
         <v>264</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G41" s="2">
         <v>43</v>
@@ -20031,10 +19476,10 @@
         <v>267</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G42" s="2">
         <v>44</v>
@@ -20052,13 +19497,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G43" s="2">
         <v>45</v>
@@ -20076,13 +19521,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D44" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G44" s="2">
         <v>46</v>
@@ -20100,13 +19545,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D45" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G45" s="2">
         <v>47</v>
@@ -20127,10 +19572,10 @@
         <v>264</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G46" s="2">
         <v>48</v>
@@ -20151,10 +19596,10 @@
         <v>267</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G47" s="2">
         <v>49</v>
@@ -20172,13 +19617,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G48" s="2">
         <v>50</v>
@@ -20196,13 +19641,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G49" s="2">
         <v>51</v>
@@ -20223,10 +19668,10 @@
         <v>264</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G50" s="2">
         <v>52</v>
@@ -20247,10 +19692,10 @@
         <v>267</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G51" s="2">
         <v>53</v>
@@ -20268,13 +19713,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D52" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G52" s="2">
         <v>54</v>
@@ -20292,13 +19737,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D53" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G53" s="2">
         <v>55</v>
@@ -20316,13 +19761,13 @@
         <v>Proponent must submit a Revised DPD</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="G54" s="2">
         <v>56</v>
@@ -20343,10 +19788,10 @@
         <v>258</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G55" s="2">
         <v>58</v>
@@ -20367,10 +19812,10 @@
         <v>258</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G56" s="2">
         <v>59</v>
@@ -20388,13 +19833,13 @@
         <v>Project is Referred to Minister for Termination</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G57" s="2">
         <v>60</v>
@@ -20415,10 +19860,10 @@
         <v>261</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G58" s="2">
         <v>61</v>
@@ -20439,10 +19884,10 @@
         <v>270</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G59" s="2">
         <v>63</v>
@@ -20463,10 +19908,10 @@
         <v>258</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G60" s="2">
         <v>64</v>
@@ -20487,10 +19932,10 @@
         <v>258</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G61" s="2">
         <v>65</v>
@@ -20511,10 +19956,10 @@
         <v>264</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G62" s="2">
         <v>67</v>
@@ -20535,10 +19980,10 @@
         <v>267</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G63" s="2">
         <v>68</v>
@@ -20556,13 +20001,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G64" s="2">
         <v>69</v>
@@ -20580,13 +20025,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D65" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G65" s="2">
         <v>70</v>
@@ -20607,10 +20052,10 @@
         <v>264</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G66" s="2">
         <v>71</v>
@@ -20631,10 +20076,10 @@
         <v>267</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G67" s="2">
         <v>72</v>
@@ -20652,13 +20097,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D68" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G68" s="2">
         <v>73</v>
@@ -20676,13 +20121,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D69" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G69" s="2">
         <v>74</v>
@@ -20703,10 +20148,10 @@
         <v>264</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G70" s="2">
         <v>75</v>
@@ -20727,10 +20172,10 @@
         <v>267</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G71" s="2">
         <v>76</v>
@@ -20748,13 +20193,13 @@
         <v>Project is Terminated</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G72" s="2">
         <v>77</v>
@@ -20772,13 +20217,13 @@
         <v>Project is Terminated</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G73" s="2">
         <v>78</v>
@@ -20796,13 +20241,13 @@
         <v>Refer the Project to the CEAO for Further Decision</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G74" s="2">
         <v>79</v>
@@ -20823,10 +20268,10 @@
         <v>258</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G75" s="2">
         <v>80</v>
@@ -20847,10 +20292,10 @@
         <v>264</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G76" s="2">
         <v>81</v>
@@ -20871,10 +20316,10 @@
         <v>267</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G77" s="2">
         <v>82</v>
@@ -20892,13 +20337,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G78" s="2">
         <v>83</v>
@@ -20916,13 +20361,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D79" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G79" s="2">
         <v>84</v>
@@ -20943,10 +20388,10 @@
         <v>264</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G80" s="2">
         <v>85</v>
@@ -20967,10 +20412,10 @@
         <v>267</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G81" s="2">
         <v>86</v>
@@ -20988,13 +20433,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D82" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G82" s="2">
         <v>87</v>
@@ -21012,13 +20457,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D83" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G83" s="2">
         <v>88</v>
@@ -21036,13 +20481,13 @@
         <v>Proponent must submit a Revised DPD</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="G84" s="2">
         <v>89</v>
@@ -21063,10 +20508,10 @@
         <v>258</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G85" s="2">
         <v>91</v>
@@ -21087,10 +20532,10 @@
         <v>258</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G86" s="2">
         <v>92</v>
@@ -21108,13 +20553,13 @@
         <v>Set federalInvolvement to "None"</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>243</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G87" s="2">
         <v>94</v>
@@ -21132,13 +20577,13 @@
         <v>Set federalInvolvement to "None"</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>243</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G88" s="2">
         <v>96</v>
@@ -21156,13 +20601,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G89" s="2">
         <v>97</v>
@@ -21183,10 +20628,10 @@
         <v>264</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G90" s="2">
         <v>98</v>
@@ -21207,10 +20652,10 @@
         <v>267</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G91" s="2">
         <v>99</v>
@@ -21228,13 +20673,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G92" s="2">
         <v>100</v>
@@ -21252,13 +20697,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D93" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G93" s="2">
         <v>101</v>
@@ -21279,10 +20724,10 @@
         <v>264</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G94" s="2">
         <v>102</v>
@@ -21303,10 +20748,10 @@
         <v>267</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G95" s="2">
         <v>103</v>
@@ -21324,13 +20769,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D96" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G96" s="2">
         <v>104</v>
@@ -21348,13 +20793,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D97" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G97" s="2">
         <v>105</v>
@@ -21375,10 +20820,10 @@
         <v>258</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G98" s="2">
         <v>106</v>
@@ -21399,10 +20844,10 @@
         <v>258</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G99" s="2">
         <v>107</v>
@@ -21423,10 +20868,10 @@
         <v>261</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G100" s="2">
         <v>108</v>
@@ -21444,13 +20889,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D101" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G101" s="2">
         <v>110</v>
@@ -21471,10 +20916,10 @@
         <v>264</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G102" s="2">
         <v>111</v>
@@ -21495,10 +20940,10 @@
         <v>267</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G103" s="2">
         <v>112</v>
@@ -21516,13 +20961,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G104" s="2">
         <v>113</v>
@@ -21540,13 +20985,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D105" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G105" s="2">
         <v>114</v>
@@ -21567,10 +21012,10 @@
         <v>264</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G106" s="2">
         <v>115</v>
@@ -21591,10 +21036,10 @@
         <v>267</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G107" s="2">
         <v>116</v>
@@ -21612,13 +21057,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D108" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G108" s="2">
         <v>117</v>
@@ -21636,13 +21081,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D109" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G109" s="2">
         <v>118</v>
@@ -21660,13 +21105,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D110" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G110" s="2">
         <v>119</v>
@@ -21687,10 +21132,10 @@
         <v>264</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G111" s="2">
         <v>120</v>
@@ -21711,10 +21156,10 @@
         <v>267</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G112" s="2">
         <v>121</v>
@@ -21732,13 +21177,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G113" s="2">
         <v>122</v>
@@ -21756,13 +21201,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D114" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G114" s="2">
         <v>123</v>
@@ -21783,10 +21228,10 @@
         <v>264</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G115" s="2">
         <v>124</v>
@@ -21807,10 +21252,10 @@
         <v>267</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G116" s="2">
         <v>125</v>
@@ -21828,13 +21273,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D117" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G117" s="2">
         <v>126</v>
@@ -21852,13 +21297,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D118" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G118" s="2">
         <v>127</v>
@@ -21879,10 +21324,10 @@
         <v>258</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G119" s="2">
         <v>128</v>
@@ -21903,10 +21348,10 @@
         <v>258</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G120" s="2">
         <v>129</v>
@@ -21927,10 +21372,10 @@
         <v>261</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G121" s="2">
         <v>130</v>
@@ -21948,13 +21393,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D122" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G122" s="2">
         <v>132</v>
@@ -21975,10 +21420,10 @@
         <v>264</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G123" s="2">
         <v>133</v>
@@ -21999,10 +21444,10 @@
         <v>267</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G124" s="2">
         <v>134</v>
@@ -22020,13 +21465,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G125" s="2">
         <v>135</v>
@@ -22044,13 +21489,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D126" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E126" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G126" s="2">
         <v>136</v>
@@ -22071,10 +21516,10 @@
         <v>264</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G127" s="2">
         <v>137</v>
@@ -22095,10 +21540,10 @@
         <v>267</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G128" s="2">
         <v>138</v>
@@ -22116,13 +21561,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D129" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F129" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G129" s="2">
         <v>139</v>
@@ -22140,13 +21585,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D130" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E130" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G130" s="2">
         <v>140</v>
@@ -22164,13 +21609,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D131" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F131" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G131" s="2">
         <v>141</v>
@@ -22191,10 +21636,10 @@
         <v>264</v>
       </c>
       <c r="E132" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G132" s="2">
         <v>142</v>
@@ -22215,10 +21660,10 @@
         <v>267</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G133" s="2">
         <v>143</v>
@@ -22236,13 +21681,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G134" s="2">
         <v>144</v>
@@ -22260,13 +21705,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D135" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F135" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G135" s="2">
         <v>145</v>
@@ -22287,10 +21732,10 @@
         <v>264</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G136" s="2">
         <v>146</v>
@@ -22311,10 +21756,10 @@
         <v>267</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G137" s="2">
         <v>147</v>
@@ -22332,13 +21777,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F138" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G138" s="2">
         <v>148</v>
@@ -22356,13 +21801,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D139" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F139" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G139" s="2">
         <v>149</v>
@@ -22383,10 +21828,10 @@
         <v>258</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G140" s="2">
         <v>150</v>
@@ -22407,10 +21852,10 @@
         <v>264</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G141" s="2">
         <v>151</v>
@@ -22431,10 +21876,10 @@
         <v>267</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G142" s="2">
         <v>152</v>
@@ -22452,13 +21897,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D143" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G143" s="2">
         <v>153</v>
@@ -22476,13 +21921,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D144" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E144" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G144" s="2">
         <v>154</v>
@@ -22500,13 +21945,13 @@
         <v>Environmental Assessment Certificate GRANTED</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G145" s="2">
         <v>155</v>
@@ -22524,13 +21969,13 @@
         <v>Environmental Assessment Certificate GRANTED</v>
       </c>
       <c r="D146" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F146" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="G146" s="2">
         <v>156</v>
@@ -22548,13 +21993,13 @@
         <v>Environmental Assessment Certificate REFUSED</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E147" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G147" s="2">
         <v>157</v>
@@ -22572,13 +22017,13 @@
         <v>Environmental Assessment Certificate REFUSED</v>
       </c>
       <c r="D148" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E148" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G148" s="2">
         <v>158</v>
@@ -23437,63 +22882,67 @@
       <c r="G290" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B290">
-      <formula1>Outcomes!$A$2:$A$62</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$62</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B290</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
-    <tabColor theme="7" tint="0.799981688894314"/>
+    <tabColor theme="7" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.6285714285714" style="5" customWidth="1"/>
-    <col min="3" max="3" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.6285714285714" style="5" customWidth="1"/>
-    <col min="7" max="7" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.6285714285714" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24.6285714285714" style="5" customWidth="1"/>
-    <col min="10" max="10" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.6285714285714" style="5" customWidth="1"/>
-    <col min="12" max="12" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.6285714285714" style="5" customWidth="1"/>
-    <col min="14" max="14" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="15" max="15" width="30.6285714285714" style="5" customWidth="1"/>
-    <col min="16" max="16" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="17" max="17" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="18" max="18" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="19" max="19" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="20" max="58" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="59" max="59" width="8.90476190476191" style="5"/>
-    <col min="60" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="3.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="3.6328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="3.6328125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="3.6328125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="3.6328125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="30.6328125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="3.6328125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="14.6328125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="3.6328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" style="5" customWidth="1"/>
+    <col min="20" max="58" width="3.6328125" style="5" customWidth="1"/>
+    <col min="59" max="59" width="8.90625" style="5"/>
+    <col min="60" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1"/>
-    <row r="2" s="6" customFormat="1" spans="1:59">
+    <row r="1" spans="1:59" s="5" customFormat="1"/>
+    <row r="2" spans="1:59" s="6" customFormat="1">
       <c r="A2" s="7"/>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="6" t="s">
@@ -23502,11 +22951,11 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
@@ -23518,11 +22967,11 @@
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R2" s="7"/>
       <c r="S2" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
@@ -23565,9 +23014,9 @@
       <c r="BF2" s="7"/>
       <c r="BG2" s="7"/>
     </row>
-    <row r="3" spans="2:19">
+    <row r="3" spans="1:59">
       <c r="B3" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
@@ -23588,7 +23037,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>56</v>
@@ -23597,12 +23046,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="1:59">
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -23620,21 +23069,21 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59">
+      <c r="B5" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>55</v>
@@ -23646,15 +23095,15 @@
         <v>41</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>55</v>
@@ -23666,12 +23115,12 @@
         <v>62</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59">
       <c r="B7" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>55</v>
@@ -23683,12 +23132,12 @@
         <v>93</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59">
       <c r="B8" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>55</v>
@@ -23700,12 +23149,12 @@
         <v>119</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59">
       <c r="B9" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>55</v>
@@ -23714,15 +23163,15 @@
         <v>108</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59">
+      <c r="B10" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15">
-      <c r="B10" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>55</v>
@@ -23731,12 +23180,12 @@
         <v>67</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59">
       <c r="B11" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>55</v>
@@ -23746,9 +23195,9 @@
       </c>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="1:59">
       <c r="B12" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>55</v>
@@ -23758,9 +23207,9 @@
       </c>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="1:59">
       <c r="B13" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>119</v>
@@ -23770,9 +23219,9 @@
       </c>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="1:59">
       <c r="B14" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>119</v>
@@ -23782,27 +23231,27 @@
       </c>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="1:59">
       <c r="B15" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="1:59">
       <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="8:9">
@@ -23834,7 +23283,7 @@
         <v>41</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="8:9">
@@ -23858,7 +23307,7 @@
         <v>41</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="8:9">
@@ -23938,7 +23387,7 @@
         <v>65</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="8:9">
@@ -23970,7 +23419,7 @@
         <v>62</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="8:9">
@@ -23978,7 +23427,7 @@
         <v>62</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="8:9">
@@ -23990,38 +23439,36 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="O3:O15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:O15">
     <sortCondition ref="O3:O15"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>$K$3:$K$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="40.0857142857143" customWidth="1"/>
-    <col min="4" max="4" width="10.8190476190476" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="2">
         <v>3</v>
       </c>
@@ -24033,35 +23480,40 @@
         <v>Project Transitioning FROM the EA Act (2002)</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E1" s="2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>Events!$A$2:$A$319</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
+          <x14:formula1>
+            <xm:f>Events!$A$2:$A$319</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="$A4:$XFD4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2">
         <v>4</v>
       </c>
@@ -24073,19 +23525,19 @@
         <v>#N/A</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G1" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="2">
         <v>66</v>
       </c>
@@ -24097,19 +23549,19 @@
         <v>Refer for Minister's Process Planning</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G2" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:7">
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="2">
         <v>93</v>
       </c>
@@ -24121,19 +23573,19 @@
         <v>Refer for Minister's Process Planning</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G3" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:7">
+    <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="2">
         <v>95</v>
       </c>
@@ -24145,25 +23597,31 @@
         <v>Unknown QQQ (how to set federalInvolvement properly)</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G4" s="2">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B4">
-      <formula1>Outcomes!$A$2:$A$62</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$62</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Template name fixes + Change phase event implementation (#1921)
* template import issue fix

* fix

* template fixes and change_phase_end_event action changes

* ceao designation revert changes

* lint fixes

* test fixes

* test fixes

* test fixes
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/001_EAC_Assessment.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08BAA25-8016-4D80-8F37-BFA98CAB2D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="14400" windowHeight="12945" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -20,7 +26,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Events!$A$1:$N$319</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outcomes!$A$1:$E$62</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1027,12 +1046,6 @@
     <t>ChangePhaseEndEvent</t>
   </si>
   <si>
-    <t>Set "Early Engagement | Project Transitioning FROM the EA Act (2002)" to PHASE END EVENT</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "Project Transitioning FROM the EA Act (2002)"}</t>
-  </si>
-  <si>
     <t>Set "DPD Development (Proponent Time) | Start of Detailed Project Description Development" ACTUAL to thisEventActual +1</t>
   </si>
   <si>
@@ -1376,19 +1389,19 @@
   </si>
   <si>
     <t>We currently don’t know how to handle this in EPIC.track</t>
+  </si>
+  <si>
+    <t>Set "Pre-Early Engagement | Project Transitioning FROM the EA Act (2002)" to PHASE END EVENT</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Pre-Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "Project Transitioning FROM the EA Act (2002)"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="27">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1426,150 +1439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1595,7 +1464,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1604,19 +1473,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,13 +1497,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1667,170 +1536,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1882,253 +1589,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2261,65 +1726,29 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <color theme="0"/>
       </font>
@@ -2329,28 +1758,19 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00CCFFCC"/>
+      <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2608,26 +2028,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor theme="9" tint="0.799981688894314"/>
+    <tabColor theme="9" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.62857142857143" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="21" spans="2:2">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
@@ -2650,62 +2069,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" ht="21" spans="2:2">
+    <row r="8" spans="2:3" ht="21">
       <c r="B8" s="44" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" ht="21" spans="2:2">
+    <row r="12" spans="2:3" ht="21">
       <c r="B12" s="44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="2" customWidth="1"/>
-    <col min="2" max="2" width="50.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6285714285714" style="1" customWidth="1"/>
-    <col min="4" max="5" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="8" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6285714285714" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="50.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="14.6328125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="12.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:9">
+    <row r="1" spans="1:9" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -3082,15 +2498,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:9">
       <c r="A14"/>
       <c r="B14"/>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:9">
       <c r="A15"/>
       <c r="B15"/>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:9">
       <c r="A16"/>
       <c r="B16"/>
     </row>
@@ -3863,51 +3279,61 @@
       <c r="B208"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C13">
-      <formula1>Lookups!$B$3:$B$16</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D13">
-      <formula1>Lookups!$D$3:$D$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13">
-      <formula1>Lookups!$F$3:$F$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$B$3:$B$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$D$3:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$F$3:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D164" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="2" customWidth="1"/>
-    <col min="2" max="3" width="10.6285714285714" style="2" customWidth="1"/>
-    <col min="4" max="4" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6285714285714" style="1" customWidth="1"/>
-    <col min="7" max="9" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6285714285714" style="1" customWidth="1"/>
-    <col min="11" max="12" width="14.6285714285714" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6285714285714" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="10.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="70.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6328125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="14.6328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="14.6328125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:14">
+    <row r="1" spans="1:14" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -8262,7 +7688,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="101" ht="15.75" spans="1:14">
+    <row r="101" spans="1:14">
       <c r="A101" s="2">
         <v>102</v>
       </c>
@@ -8347,7 +7773,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="103" ht="15.75" spans="1:14">
+    <row r="103" spans="1:14">
       <c r="A103" s="28">
         <v>104</v>
       </c>
@@ -9347,7 +8773,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="126" ht="15.75" spans="1:14">
+    <row r="126" spans="1:14">
       <c r="A126" s="2">
         <v>127</v>
       </c>
@@ -9389,7 +8815,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="127" ht="15.75" spans="1:14">
+    <row r="127" spans="1:14">
       <c r="A127" s="34">
         <v>128</v>
       </c>
@@ -17821,65 +17247,82 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N319">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:N319" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <conditionalFormatting sqref="H1:H319">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="between" text="END">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="END">
       <formula>NOT(ISERROR(SEARCH("END",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="between" text="START">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="START">
       <formula>NOT(ISERROR(SEARCH("START",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C319">
-      <formula1>Phases!$A$2:$A$13</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H319">
-      <formula1>Lookups!$Q$3:$Q$5</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F319">
-      <formula1>Lookups!$I$3:$I$39</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I319">
-      <formula1>Lookups!$S$3:$S$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G319">
-      <formula1>Lookups!$K$3:$K$9</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M319">
-      <formula1>Lookups!$M$3:$M$4</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Phases!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$Q$3:$Q$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$I$3:$I$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$S$3:$S$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000004000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$K$3:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G319</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000005000000}">
+          <x14:formula1>
+            <xm:f>Lookups!$M$3:$M$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M319</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="6.62857142857143" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="4" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="6.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6328125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="70.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -18995,45 +18438,47 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E62">
-    <extLst/>
-  </autoFilter>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B62">
-      <formula1>Events!$A$2:$A$319</formula1>
-    </dataValidation>
-  </dataValidations>
+  <autoFilter ref="A1:E62" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Events!$A$2:$A$319</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B62</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.90476190476191" style="1"/>
-    <col min="2" max="2" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.6285714285714" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="108.628571428571" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.6285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6285714285714" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="12.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="70.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="108.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -19167,10 +18612,10 @@
         <v>270</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G6" s="2">
         <v>7</v>
@@ -19191,10 +18636,10 @@
         <v>258</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G7" s="2">
         <v>8</v>
@@ -19215,10 +18660,10 @@
         <v>264</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G8" s="2">
         <v>9</v>
@@ -19239,10 +18684,10 @@
         <v>258</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G9" s="2">
         <v>10</v>
@@ -19263,10 +18708,10 @@
         <v>258</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G10" s="2">
         <v>11</v>
@@ -19287,10 +18732,10 @@
         <v>264</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G11" s="2">
         <v>12</v>
@@ -19335,10 +18780,10 @@
         <v>270</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G13" s="2">
         <v>14</v>
@@ -19359,10 +18804,10 @@
         <v>258</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G14" s="2">
         <v>15</v>
@@ -19383,10 +18828,10 @@
         <v>264</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G15" s="2">
         <v>16</v>
@@ -19431,10 +18876,10 @@
         <v>270</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>272</v>
+        <v>387</v>
       </c>
       <c r="G17" s="2">
         <v>18</v>
@@ -19455,10 +18900,10 @@
         <v>258</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G18" s="2">
         <v>19</v>
@@ -19479,10 +18924,10 @@
         <v>264</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G19" s="2">
         <v>20</v>
@@ -19503,10 +18948,10 @@
         <v>267</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G20" s="2">
         <v>21</v>
@@ -19524,13 +18969,13 @@
         <v>Proponent withdraws Submission from the EAC Assessment process</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G21" s="2">
         <v>22</v>
@@ -19548,13 +18993,13 @@
         <v>Proponent withdraws Submission from the EAC Assessment process</v>
       </c>
       <c r="D22" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G22" s="2">
         <v>23</v>
@@ -19572,13 +19017,13 @@
         <v>Starts the "clock" for EAC Assessment</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="G23" s="2">
         <v>24</v>
@@ -19596,13 +19041,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G24" s="2">
         <v>25</v>
@@ -19623,10 +19068,10 @@
         <v>264</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G25" s="2">
         <v>26</v>
@@ -19647,10 +19092,10 @@
         <v>267</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G26" s="2">
         <v>27</v>
@@ -19668,13 +19113,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G27" s="2">
         <v>28</v>
@@ -19692,13 +19137,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D28" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G28" s="2">
         <v>29</v>
@@ -19719,10 +19164,10 @@
         <v>264</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G29" s="2">
         <v>30</v>
@@ -19743,10 +19188,10 @@
         <v>267</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G30" s="2">
         <v>31</v>
@@ -19764,13 +19209,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G31" s="2">
         <v>32</v>
@@ -19788,13 +19233,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D32" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G32" s="2">
         <v>33</v>
@@ -19815,10 +19260,10 @@
         <v>258</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G33" s="2">
         <v>34</v>
@@ -19839,10 +19284,10 @@
         <v>258</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G34" s="2">
         <v>35</v>
@@ -19863,10 +19308,10 @@
         <v>261</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G35" s="2">
         <v>36</v>
@@ -19884,13 +19329,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G36" s="2">
         <v>38</v>
@@ -19911,10 +19356,10 @@
         <v>264</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G37" s="2">
         <v>39</v>
@@ -19935,10 +19380,10 @@
         <v>267</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G38" s="2">
         <v>40</v>
@@ -19956,13 +19401,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G39" s="2">
         <v>41</v>
@@ -19980,13 +19425,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G40" s="2">
         <v>42</v>
@@ -20007,10 +19452,10 @@
         <v>264</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G41" s="2">
         <v>43</v>
@@ -20031,10 +19476,10 @@
         <v>267</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G42" s="2">
         <v>44</v>
@@ -20052,13 +19497,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G43" s="2">
         <v>45</v>
@@ -20076,13 +19521,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D44" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G44" s="2">
         <v>46</v>
@@ -20100,13 +19545,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D45" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G45" s="2">
         <v>47</v>
@@ -20127,10 +19572,10 @@
         <v>264</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G46" s="2">
         <v>48</v>
@@ -20151,10 +19596,10 @@
         <v>267</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G47" s="2">
         <v>49</v>
@@ -20172,13 +19617,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G48" s="2">
         <v>50</v>
@@ -20196,13 +19641,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D49" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G49" s="2">
         <v>51</v>
@@ -20223,10 +19668,10 @@
         <v>264</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G50" s="2">
         <v>52</v>
@@ -20247,10 +19692,10 @@
         <v>267</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G51" s="2">
         <v>53</v>
@@ -20268,13 +19713,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D52" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G52" s="2">
         <v>54</v>
@@ -20292,13 +19737,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D53" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G53" s="2">
         <v>55</v>
@@ -20316,13 +19761,13 @@
         <v>Proponent must submit a Revised DPD</v>
       </c>
       <c r="D54" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="G54" s="2">
         <v>56</v>
@@ -20343,10 +19788,10 @@
         <v>258</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G55" s="2">
         <v>58</v>
@@ -20367,10 +19812,10 @@
         <v>258</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G56" s="2">
         <v>59</v>
@@ -20388,13 +19833,13 @@
         <v>Project is Referred to Minister for Termination</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G57" s="2">
         <v>60</v>
@@ -20415,10 +19860,10 @@
         <v>261</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G58" s="2">
         <v>61</v>
@@ -20439,10 +19884,10 @@
         <v>270</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G59" s="2">
         <v>63</v>
@@ -20463,10 +19908,10 @@
         <v>258</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G60" s="2">
         <v>64</v>
@@ -20487,10 +19932,10 @@
         <v>258</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G61" s="2">
         <v>65</v>
@@ -20511,10 +19956,10 @@
         <v>264</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G62" s="2">
         <v>67</v>
@@ -20535,10 +19980,10 @@
         <v>267</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G63" s="2">
         <v>68</v>
@@ -20556,13 +20001,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G64" s="2">
         <v>69</v>
@@ -20580,13 +20025,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D65" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G65" s="2">
         <v>70</v>
@@ -20607,10 +20052,10 @@
         <v>264</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G66" s="2">
         <v>71</v>
@@ -20631,10 +20076,10 @@
         <v>267</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G67" s="2">
         <v>72</v>
@@ -20652,13 +20097,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D68" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G68" s="2">
         <v>73</v>
@@ -20676,13 +20121,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D69" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G69" s="2">
         <v>74</v>
@@ -20703,10 +20148,10 @@
         <v>264</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G70" s="2">
         <v>75</v>
@@ -20727,10 +20172,10 @@
         <v>267</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G71" s="2">
         <v>76</v>
@@ -20748,13 +20193,13 @@
         <v>Project is Terminated</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G72" s="2">
         <v>77</v>
@@ -20772,13 +20217,13 @@
         <v>Project is Terminated</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G73" s="2">
         <v>78</v>
@@ -20796,13 +20241,13 @@
         <v>Refer the Project to the CEAO for Further Decision</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G74" s="2">
         <v>79</v>
@@ -20823,10 +20268,10 @@
         <v>258</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G75" s="2">
         <v>80</v>
@@ -20847,10 +20292,10 @@
         <v>264</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G76" s="2">
         <v>81</v>
@@ -20871,10 +20316,10 @@
         <v>267</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G77" s="2">
         <v>82</v>
@@ -20892,13 +20337,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G78" s="2">
         <v>83</v>
@@ -20916,13 +20361,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D79" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G79" s="2">
         <v>84</v>
@@ -20943,10 +20388,10 @@
         <v>264</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G80" s="2">
         <v>85</v>
@@ -20967,10 +20412,10 @@
         <v>267</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G81" s="2">
         <v>86</v>
@@ -20988,13 +20433,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D82" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G82" s="2">
         <v>87</v>
@@ -21012,13 +20457,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D83" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G83" s="2">
         <v>88</v>
@@ -21036,13 +20481,13 @@
         <v>Proponent must submit a Revised DPD</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>312</v>
       </c>
       <c r="G84" s="2">
         <v>89</v>
@@ -21063,10 +20508,10 @@
         <v>258</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G85" s="2">
         <v>91</v>
@@ -21087,10 +20532,10 @@
         <v>258</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G86" s="2">
         <v>92</v>
@@ -21108,13 +20553,13 @@
         <v>Set federalInvolvement to "None"</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>243</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G87" s="2">
         <v>94</v>
@@ -21132,13 +20577,13 @@
         <v>Set federalInvolvement to "None"</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>243</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G88" s="2">
         <v>96</v>
@@ -21156,13 +20601,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G89" s="2">
         <v>97</v>
@@ -21183,10 +20628,10 @@
         <v>264</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G90" s="2">
         <v>98</v>
@@ -21207,10 +20652,10 @@
         <v>267</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G91" s="2">
         <v>99</v>
@@ -21228,13 +20673,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G92" s="2">
         <v>100</v>
@@ -21252,13 +20697,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D93" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G93" s="2">
         <v>101</v>
@@ -21279,10 +20724,10 @@
         <v>264</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G94" s="2">
         <v>102</v>
@@ -21303,10 +20748,10 @@
         <v>267</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G95" s="2">
         <v>103</v>
@@ -21324,13 +20769,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D96" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G96" s="2">
         <v>104</v>
@@ -21348,13 +20793,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D97" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G97" s="2">
         <v>105</v>
@@ -21375,10 +20820,10 @@
         <v>258</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G98" s="2">
         <v>106</v>
@@ -21399,10 +20844,10 @@
         <v>258</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="G99" s="2">
         <v>107</v>
@@ -21423,10 +20868,10 @@
         <v>261</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G100" s="2">
         <v>108</v>
@@ -21444,13 +20889,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D101" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F101" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G101" s="2">
         <v>110</v>
@@ -21471,10 +20916,10 @@
         <v>264</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G102" s="2">
         <v>111</v>
@@ -21495,10 +20940,10 @@
         <v>267</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G103" s="2">
         <v>112</v>
@@ -21516,13 +20961,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G104" s="2">
         <v>113</v>
@@ -21540,13 +20985,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D105" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F105" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G105" s="2">
         <v>114</v>
@@ -21567,10 +21012,10 @@
         <v>264</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G106" s="2">
         <v>115</v>
@@ -21591,10 +21036,10 @@
         <v>267</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G107" s="2">
         <v>116</v>
@@ -21612,13 +21057,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D108" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F108" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G108" s="2">
         <v>117</v>
@@ -21636,13 +21081,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D109" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F109" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G109" s="2">
         <v>118</v>
@@ -21660,13 +21105,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D110" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F110" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G110" s="2">
         <v>119</v>
@@ -21687,10 +21132,10 @@
         <v>264</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G111" s="2">
         <v>120</v>
@@ -21711,10 +21156,10 @@
         <v>267</v>
       </c>
       <c r="E112" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G112" s="2">
         <v>121</v>
@@ -21732,13 +21177,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G113" s="2">
         <v>122</v>
@@ -21756,13 +21201,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D114" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G114" s="2">
         <v>123</v>
@@ -21783,10 +21228,10 @@
         <v>264</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G115" s="2">
         <v>124</v>
@@ -21807,10 +21252,10 @@
         <v>267</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G116" s="2">
         <v>125</v>
@@ -21828,13 +21273,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D117" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E117" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G117" s="2">
         <v>126</v>
@@ -21852,13 +21297,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D118" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G118" s="2">
         <v>127</v>
@@ -21879,10 +21324,10 @@
         <v>258</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G119" s="2">
         <v>128</v>
@@ -21903,10 +21348,10 @@
         <v>258</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G120" s="2">
         <v>129</v>
@@ -21927,10 +21372,10 @@
         <v>261</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G121" s="2">
         <v>130</v>
@@ -21948,13 +21393,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D122" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G122" s="2">
         <v>132</v>
@@ -21975,10 +21420,10 @@
         <v>264</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G123" s="2">
         <v>133</v>
@@ -21999,10 +21444,10 @@
         <v>267</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G124" s="2">
         <v>134</v>
@@ -22020,13 +21465,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D125" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G125" s="2">
         <v>135</v>
@@ -22044,13 +21489,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D126" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F126" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E126" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F126" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G126" s="2">
         <v>136</v>
@@ -22071,10 +21516,10 @@
         <v>264</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G127" s="2">
         <v>137</v>
@@ -22095,10 +21540,10 @@
         <v>267</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G128" s="2">
         <v>138</v>
@@ -22116,13 +21561,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D129" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F129" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E129" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G129" s="2">
         <v>139</v>
@@ -22140,13 +21585,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D130" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F130" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E130" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G130" s="2">
         <v>140</v>
@@ -22164,13 +21609,13 @@
         <v>Dispute Resolution is started</v>
       </c>
       <c r="D131" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F131" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="E131" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="G131" s="2">
         <v>141</v>
@@ -22191,10 +21636,10 @@
         <v>264</v>
       </c>
       <c r="E132" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G132" s="2">
         <v>142</v>
@@ -22215,10 +21660,10 @@
         <v>267</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G133" s="2">
         <v>143</v>
@@ -22236,13 +21681,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D134" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G134" s="2">
         <v>144</v>
@@ -22260,13 +21705,13 @@
         <v>EAC Assessment is Terminated under s.39(d) of Act</v>
       </c>
       <c r="D135" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F135" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E135" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G135" s="2">
         <v>145</v>
@@ -22287,10 +21732,10 @@
         <v>264</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G136" s="2">
         <v>146</v>
@@ -22311,10 +21756,10 @@
         <v>267</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G137" s="2">
         <v>147</v>
@@ -22332,13 +21777,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F138" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E138" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G138" s="2">
         <v>148</v>
@@ -22356,13 +21801,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D139" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F139" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G139" s="2">
         <v>149</v>
@@ -22383,10 +21828,10 @@
         <v>258</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G140" s="2">
         <v>150</v>
@@ -22407,10 +21852,10 @@
         <v>264</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G141" s="2">
         <v>151</v>
@@ -22431,10 +21876,10 @@
         <v>267</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G142" s="2">
         <v>152</v>
@@ -22452,13 +21897,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D143" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="G143" s="2">
         <v>153</v>
@@ -22476,13 +21921,13 @@
         <v>Proponent withdraws Project from EA process</v>
       </c>
       <c r="D144" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F144" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E144" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G144" s="2">
         <v>154</v>
@@ -22500,13 +21945,13 @@
         <v>Environmental Assessment Certificate GRANTED</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G145" s="2">
         <v>155</v>
@@ -22524,13 +21969,13 @@
         <v>Environmental Assessment Certificate GRANTED</v>
       </c>
       <c r="D146" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="F146" s="1" t="s">
         <v>346</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="G146" s="2">
         <v>156</v>
@@ -22548,13 +21993,13 @@
         <v>Environmental Assessment Certificate REFUSED</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E147" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G147" s="2">
         <v>157</v>
@@ -22572,13 +22017,13 @@
         <v>Environmental Assessment Certificate REFUSED</v>
       </c>
       <c r="D148" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="E148" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="G148" s="2">
         <v>158</v>
@@ -23437,63 +22882,67 @@
       <c r="G290" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B290">
-      <formula1>Outcomes!$A$2:$A$62</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$62</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B290</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
-    <tabColor theme="7" tint="0.799981688894314"/>
+    <tabColor theme="7" tint="0.79995117038483843"/>
   </sheetPr>
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.6285714285714" style="5" customWidth="1"/>
-    <col min="3" max="3" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="5" max="5" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="6" max="6" width="12.6285714285714" style="5" customWidth="1"/>
-    <col min="7" max="7" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="8" max="8" width="10.6285714285714" style="5" customWidth="1"/>
-    <col min="9" max="9" width="24.6285714285714" style="5" customWidth="1"/>
-    <col min="10" max="10" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.6285714285714" style="5" customWidth="1"/>
-    <col min="12" max="12" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="13" max="13" width="12.6285714285714" style="5" customWidth="1"/>
-    <col min="14" max="14" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="15" max="15" width="30.6285714285714" style="5" customWidth="1"/>
-    <col min="16" max="16" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="17" max="17" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="18" max="18" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="19" max="19" width="14.6285714285714" style="5" customWidth="1"/>
-    <col min="20" max="58" width="3.62857142857143" style="5" customWidth="1"/>
-    <col min="59" max="59" width="8.90476190476191" style="5"/>
-    <col min="60" max="16384" width="8.90476190476191" style="1"/>
+    <col min="1" max="1" width="3.6328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="3.6328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.6328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="3.6328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="3.6328125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="16.6328125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="3.6328125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" style="5" customWidth="1"/>
+    <col min="14" max="14" width="3.6328125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="30.6328125" style="5" customWidth="1"/>
+    <col min="16" max="16" width="3.6328125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="14.6328125" style="5" customWidth="1"/>
+    <col min="18" max="18" width="3.6328125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="14.6328125" style="5" customWidth="1"/>
+    <col min="20" max="58" width="3.6328125" style="5" customWidth="1"/>
+    <col min="59" max="59" width="8.90625" style="5"/>
+    <col min="60" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1"/>
-    <row r="2" s="6" customFormat="1" spans="1:59">
+    <row r="1" spans="1:59" s="5" customFormat="1"/>
+    <row r="2" spans="1:59" s="6" customFormat="1">
       <c r="A2" s="7"/>
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="6" t="s">
@@ -23502,11 +22951,11 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="6" t="s">
@@ -23518,11 +22967,11 @@
       </c>
       <c r="P2" s="7"/>
       <c r="Q2" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="R2" s="7"/>
       <c r="S2" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
@@ -23565,9 +23014,9 @@
       <c r="BF2" s="7"/>
       <c r="BG2" s="7"/>
     </row>
-    <row r="3" spans="2:19">
+    <row r="3" spans="1:59">
       <c r="B3" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>20</v>
@@ -23588,7 +23037,7 @@
         <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>56</v>
@@ -23597,12 +23046,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:19">
+    <row r="4" spans="1:59">
       <c r="B4" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F4" s="1" t="b">
         <v>0</v>
@@ -23620,21 +23069,21 @@
         <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59">
+      <c r="B5" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>358</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S4" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="B5" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>55</v>
@@ -23646,15 +23095,15 @@
         <v>41</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="Q5" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>55</v>
@@ -23666,12 +23115,12 @@
         <v>62</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59">
       <c r="B7" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>55</v>
@@ -23683,12 +23132,12 @@
         <v>93</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="8" spans="1:59">
       <c r="B8" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>55</v>
@@ -23700,12 +23149,12 @@
         <v>119</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:59">
       <c r="B9" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>55</v>
@@ -23714,15 +23163,15 @@
         <v>108</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59">
+      <c r="B10" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15">
-      <c r="B10" s="1" t="s">
-        <v>371</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>55</v>
@@ -23731,12 +23180,12 @@
         <v>67</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59">
       <c r="B11" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>55</v>
@@ -23746,9 +23195,9 @@
       </c>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="1:59">
       <c r="B12" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>55</v>
@@ -23758,9 +23207,9 @@
       </c>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="1:59">
       <c r="B13" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>119</v>
@@ -23770,9 +23219,9 @@
       </c>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="1:59">
       <c r="B14" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>119</v>
@@ -23782,27 +23231,27 @@
       </c>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="1:59">
       <c r="B15" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="1:59">
       <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="8:9">
@@ -23834,7 +23283,7 @@
         <v>41</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="8:9">
@@ -23858,7 +23307,7 @@
         <v>41</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="8:9">
@@ -23938,7 +23387,7 @@
         <v>65</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="8:9">
@@ -23970,7 +23419,7 @@
         <v>62</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="8:9">
@@ -23978,7 +23427,7 @@
         <v>62</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="8:9">
@@ -23990,38 +23439,36 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="O3:O15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O3:O15">
     <sortCondition ref="O3:O15"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H39" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>$K$3:$K$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="40.0857142857143" customWidth="1"/>
-    <col min="4" max="4" width="10.8190476190476" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="2">
         <v>3</v>
       </c>
@@ -24033,35 +23480,40 @@
         <v>Project Transitioning FROM the EA Act (2002)</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E1" s="2">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>Events!$A$2:$A$319</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
+          <x14:formula1>
+            <xm:f>Events!$A$2:$A$319</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="$A4:$XFD4"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="2">
         <v>4</v>
       </c>
@@ -24073,19 +23525,19 @@
         <v>#N/A</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G1" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="2">
         <v>66</v>
       </c>
@@ -24097,19 +23549,19 @@
         <v>Refer for Minister's Process Planning</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G2" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:7">
+    <row r="3" spans="1:7" s="1" customFormat="1">
       <c r="A3" s="2">
         <v>93</v>
       </c>
@@ -24121,19 +23573,19 @@
         <v>Refer for Minister's Process Planning</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G3" s="2">
         <v>93</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:7">
+    <row r="4" spans="1:7" s="1" customFormat="1">
       <c r="A4" s="2">
         <v>95</v>
       </c>
@@ -24145,25 +23597,31 @@
         <v>Unknown QQQ (how to set federalInvolvement properly)</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G4" s="2">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B4">
-      <formula1>Outcomes!$A$2:$A$62</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0700-000000000000}">
+          <x14:formula1>
+            <xm:f>Outcomes!$A$2:$A$62</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>